<commit_message>
Updated code to incorporate log-transformed flame duration into map figure. Some file reorganization and renaming.
</commit_message>
<xml_diff>
--- a/manuscript/tables/Table1.xlsx
+++ b/manuscript/tables/Table1.xlsx
@@ -1,22 +1,23 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="10410"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="11209"/>
   <workbookPr date1904="1" showInkAnnotation="0" autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Jens/Documents/Davis/Post-Doc/FireTraits/fire_traits/manuscript/tables/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jtstevens/Documents/Davis/Post-Doc/FireTraits/fire_traits/manuscript/tables/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{A38D8A68-C819-6A45-95F9-220D9BB2172C}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C209C924-E24A-D34E-9B14-4048082FA169}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="14660" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="800" yWindow="460" windowWidth="25600" windowHeight="14660" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Table1" sheetId="1" r:id="rId1"/>
-    <sheet name="tmp" sheetId="6" r:id="rId2"/>
+    <sheet name="Table1_10_21_18" sheetId="7" r:id="rId2"/>
+    <sheet name="tmp" sheetId="6" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="181029"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
@@ -26,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="108" uniqueCount="73">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="152" uniqueCount="74">
   <si>
     <t>Scientific_Name</t>
   </si>
@@ -250,6 +251,7 @@
         <sz val="10"/>
         <color rgb="FF000000"/>
         <rFont val="Times New Roman"/>
+        <family val="1"/>
       </rPr>
       <t>1</t>
     </r>
@@ -264,6 +266,7 @@
         <sz val="10"/>
         <color rgb="FF000000"/>
         <rFont val="Times New Roman"/>
+        <family val="1"/>
       </rPr>
       <t>2</t>
     </r>
@@ -272,8 +275,24 @@
         <sz val="10"/>
         <color rgb="FF000000"/>
         <rFont val="Times New Roman"/>
+        <family val="1"/>
       </rPr>
       <t xml:space="preserve"> of fh and pc</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>Flame duration</t>
+    </r>
+    <r>
+      <rPr>
+        <vertAlign val="subscript"/>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t>3</t>
     </r>
   </si>
 </sst>
@@ -285,7 +304,7 @@
     <numFmt numFmtId="164" formatCode="_-&quot;$&quot;* #,##0.00_-;\-&quot;$&quot;* #,##0.00_-;_-&quot;$&quot;* &quot;-&quot;??_-;_-@_-"/>
     <numFmt numFmtId="165" formatCode="0.0"/>
   </numFmts>
-  <fonts count="9">
+  <fonts count="9" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -313,18 +332,21 @@
       <sz val="10"/>
       <color theme="1"/>
       <name val="Times New Roman"/>
+      <family val="1"/>
     </font>
     <font>
       <b/>
       <sz val="10"/>
       <color theme="1"/>
       <name val="Times New Roman"/>
+      <family val="1"/>
     </font>
     <font>
       <i/>
       <sz val="10"/>
       <color theme="1"/>
       <name val="Times New Roman"/>
+      <family val="1"/>
     </font>
     <font>
       <sz val="10"/>
@@ -337,12 +359,14 @@
       <sz val="10"/>
       <color rgb="FF000000"/>
       <name val="Times New Roman"/>
+      <family val="1"/>
     </font>
     <font>
       <vertAlign val="subscript"/>
       <sz val="10"/>
       <color rgb="FF000000"/>
       <name val="Times New Roman"/>
+      <family val="1"/>
     </font>
   </fonts>
   <fills count="2">
@@ -353,7 +377,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -367,6 +391,17 @@
       <top/>
       <bottom style="thin">
         <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
       </bottom>
       <diagonal/>
     </border>
@@ -410,7 +445,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="19">
+  <cellXfs count="20">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
@@ -421,12 +456,6 @@
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="164" fontId="4" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -448,12 +477,21 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
   </cellXfs>
@@ -834,10 +872,10 @@
   <dimension ref="A1:W31"/>
   <sheetViews>
     <sheetView tabSelected="1" showRuler="0" workbookViewId="0">
-      <selection activeCell="Q2" sqref="Q2"/>
+      <selection sqref="A1:N31"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="21.33203125" customWidth="1"/>
     <col min="2" max="2" width="7.83203125" customWidth="1"/>
@@ -854,27 +892,27 @@
     <col min="14" max="14" width="5.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:23" ht="17">
+    <row r="1" spans="1:23" ht="17" x14ac:dyDescent="0.25">
       <c r="A1" s="1"/>
-      <c r="B1" s="14" t="s">
+      <c r="B1" s="17" t="s">
         <v>71</v>
       </c>
-      <c r="C1" s="15"/>
-      <c r="D1" s="15"/>
-      <c r="E1" s="15"/>
-      <c r="F1" s="15"/>
-      <c r="G1" s="15"/>
+      <c r="C1" s="18"/>
+      <c r="D1" s="18"/>
+      <c r="E1" s="18"/>
+      <c r="F1" s="18"/>
+      <c r="G1" s="18"/>
       <c r="H1" s="5"/>
-      <c r="I1" s="6" t="s">
+      <c r="I1" s="15" t="s">
         <v>36</v>
       </c>
-      <c r="J1" s="6"/>
-      <c r="K1" s="6"/>
-      <c r="L1" s="6"/>
-      <c r="M1" s="7"/>
+      <c r="J1" s="15"/>
+      <c r="K1" s="15"/>
+      <c r="L1" s="15"/>
+      <c r="M1" s="16"/>
       <c r="N1" s="1"/>
     </row>
-    <row r="2" spans="1:23" ht="33" customHeight="1">
+    <row r="2" spans="1:23" ht="33" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>70</v>
       </c>
@@ -906,36 +944,36 @@
       <c r="K2" s="3" t="s">
         <v>28</v>
       </c>
-      <c r="L2" s="18" t="s">
+      <c r="L2" s="19" t="s">
         <v>72</v>
       </c>
-      <c r="M2" s="3" t="s">
-        <v>29</v>
-      </c>
-      <c r="N2" s="8" t="s">
+      <c r="M2" s="19" t="s">
+        <v>73</v>
+      </c>
+      <c r="N2" s="6" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="3" spans="1:23">
-      <c r="A3" s="11" t="s">
+    <row r="3" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="A3" s="9" t="s">
         <v>64</v>
       </c>
       <c r="B3" s="4">
         <v>2.06</v>
       </c>
-      <c r="C3" s="9">
+      <c r="C3" s="7">
         <v>95.2</v>
       </c>
-      <c r="D3" s="10">
+      <c r="D3" s="8">
         <v>5</v>
       </c>
-      <c r="E3" s="9">
+      <c r="E3" s="7">
         <v>59.4</v>
       </c>
-      <c r="F3" s="9">
+      <c r="F3" s="7">
         <v>86.1</v>
       </c>
-      <c r="G3" s="9">
+      <c r="G3" s="7">
         <v>73.400000000000006</v>
       </c>
       <c r="H3" s="4"/>
@@ -952,32 +990,32 @@
         <v>0.85</v>
       </c>
       <c r="M3" s="4">
-        <v>0.94</v>
+        <v>0.87</v>
       </c>
       <c r="N3" s="4">
-        <v>0.85</v>
-      </c>
-    </row>
-    <row r="4" spans="1:23">
-      <c r="A4" s="11" t="s">
+        <v>0.83</v>
+      </c>
+    </row>
+    <row r="4" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="A4" s="9" t="s">
         <v>59</v>
       </c>
       <c r="B4" s="4">
         <v>1.73</v>
       </c>
-      <c r="C4" s="9">
+      <c r="C4" s="7">
         <v>51.4</v>
       </c>
-      <c r="D4" s="10">
+      <c r="D4" s="8">
         <v>10</v>
       </c>
-      <c r="E4" s="9">
+      <c r="E4" s="7">
         <v>67.3</v>
       </c>
-      <c r="F4" s="9">
+      <c r="F4" s="7">
         <v>90</v>
       </c>
-      <c r="G4" s="9">
+      <c r="G4" s="7">
         <v>79.2</v>
       </c>
       <c r="H4" s="4"/>
@@ -994,32 +1032,32 @@
         <v>0.93</v>
       </c>
       <c r="M4" s="4">
-        <v>0.91</v>
+        <v>0.82</v>
       </c>
       <c r="N4" s="4">
-        <v>0.82</v>
-      </c>
-    </row>
-    <row r="5" spans="1:23">
-      <c r="A5" s="11" t="s">
+        <v>0.8</v>
+      </c>
+    </row>
+    <row r="5" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="A5" s="9" t="s">
         <v>62</v>
       </c>
       <c r="B5" s="4">
         <v>1.6</v>
       </c>
-      <c r="C5" s="9">
+      <c r="C5" s="7">
         <v>41.2</v>
       </c>
-      <c r="D5" s="10">
+      <c r="D5" s="8">
         <v>10</v>
       </c>
-      <c r="E5" s="9">
+      <c r="E5" s="7">
         <v>77</v>
       </c>
-      <c r="F5" s="9">
+      <c r="F5" s="7">
         <v>92</v>
       </c>
-      <c r="G5" s="9">
+      <c r="G5" s="7">
         <v>79.7</v>
       </c>
       <c r="H5" s="4"/>
@@ -1036,123 +1074,123 @@
         <v>1</v>
       </c>
       <c r="M5" s="4">
-        <v>0.9</v>
+        <v>0.81</v>
       </c>
       <c r="N5" s="4">
-        <v>0.79</v>
-      </c>
-    </row>
-    <row r="6" spans="1:23">
-      <c r="A6" s="11" t="s">
-        <v>65</v>
+        <v>0.77</v>
+      </c>
+    </row>
+    <row r="6" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="A6" s="9" t="s">
+        <v>60</v>
       </c>
       <c r="B6" s="4">
-        <v>2.06</v>
-      </c>
-      <c r="C6" s="9">
-        <v>85.6</v>
-      </c>
-      <c r="D6" s="10">
-        <v>8</v>
-      </c>
-      <c r="E6" s="9">
-        <v>42.6</v>
-      </c>
-      <c r="F6" s="9">
-        <v>75.8</v>
-      </c>
-      <c r="G6" s="9">
-        <v>148.5</v>
+        <v>1.83</v>
+      </c>
+      <c r="C6" s="7">
+        <v>62.3</v>
+      </c>
+      <c r="D6" s="8">
+        <v>10</v>
+      </c>
+      <c r="E6" s="7">
+        <v>55.6</v>
+      </c>
+      <c r="F6" s="7">
+        <v>77.099999999999994</v>
+      </c>
+      <c r="G6" s="7">
+        <v>128.5</v>
       </c>
       <c r="H6" s="4"/>
       <c r="I6" s="4">
+        <v>0.85</v>
+      </c>
+      <c r="J6" s="4">
+        <v>0.61</v>
+      </c>
+      <c r="K6" s="4">
         <v>1</v>
       </c>
-      <c r="J6" s="4">
-        <v>0.89</v>
-      </c>
-      <c r="K6" s="4">
-        <v>0.78</v>
-      </c>
       <c r="L6" s="4">
-        <v>0.67</v>
+        <v>0.76</v>
       </c>
       <c r="M6" s="4">
-        <v>0.55000000000000004</v>
+        <v>0.48</v>
       </c>
       <c r="N6" s="4">
-        <v>0.78</v>
-      </c>
-      <c r="Q6" s="12"/>
-    </row>
-    <row r="7" spans="1:23">
-      <c r="A7" s="11" t="s">
-        <v>60</v>
+        <v>0.74</v>
+      </c>
+      <c r="Q6" s="10"/>
+    </row>
+    <row r="7" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="A7" s="9" t="s">
+        <v>65</v>
       </c>
       <c r="B7" s="4">
-        <v>1.83</v>
-      </c>
-      <c r="C7" s="9">
-        <v>62.3</v>
-      </c>
-      <c r="D7" s="10">
-        <v>10</v>
-      </c>
-      <c r="E7" s="9">
-        <v>55.6</v>
-      </c>
-      <c r="F7" s="9">
-        <v>77.099999999999994</v>
-      </c>
-      <c r="G7" s="9">
-        <v>128.5</v>
+        <v>2.06</v>
+      </c>
+      <c r="C7" s="7">
+        <v>85.6</v>
+      </c>
+      <c r="D7" s="8">
+        <v>8</v>
+      </c>
+      <c r="E7" s="7">
+        <v>42.6</v>
+      </c>
+      <c r="F7" s="7">
+        <v>75.8</v>
+      </c>
+      <c r="G7" s="7">
+        <v>148.5</v>
       </c>
       <c r="H7" s="4"/>
       <c r="I7" s="4">
-        <v>0.85</v>
+        <v>1</v>
       </c>
       <c r="J7" s="4">
-        <v>0.61</v>
+        <v>0.89</v>
       </c>
       <c r="K7" s="4">
-        <v>1</v>
+        <v>0.78</v>
       </c>
       <c r="L7" s="4">
-        <v>0.76</v>
+        <v>0.67</v>
       </c>
       <c r="M7" s="4">
-        <v>0.65</v>
+        <v>0.38</v>
       </c>
       <c r="N7" s="4">
-        <v>0.77</v>
-      </c>
-      <c r="R7" s="16"/>
-      <c r="S7" s="17"/>
-      <c r="T7" s="17"/>
-      <c r="U7" s="17"/>
-      <c r="V7" s="17"/>
-      <c r="W7" s="17"/>
-    </row>
-    <row r="8" spans="1:23">
-      <c r="A8" s="11" t="s">
+        <v>0.74</v>
+      </c>
+      <c r="R7" s="12"/>
+      <c r="S7" s="13"/>
+      <c r="T7" s="13"/>
+      <c r="U7" s="13"/>
+      <c r="V7" s="13"/>
+      <c r="W7" s="13"/>
+    </row>
+    <row r="8" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="A8" s="9" t="s">
         <v>51</v>
       </c>
       <c r="B8" s="4">
         <v>1.6</v>
       </c>
-      <c r="C8" s="9">
+      <c r="C8" s="7">
         <v>51.1</v>
       </c>
-      <c r="D8" s="10">
+      <c r="D8" s="8">
         <v>9</v>
       </c>
-      <c r="E8" s="9">
+      <c r="E8" s="7">
         <v>27.9</v>
       </c>
-      <c r="F8" s="9">
+      <c r="F8" s="7">
         <v>34.6</v>
       </c>
-      <c r="G8" s="9">
+      <c r="G8" s="7">
         <v>89.9</v>
       </c>
       <c r="H8" s="4"/>
@@ -1169,33 +1207,33 @@
         <v>0.27</v>
       </c>
       <c r="M8" s="4">
-        <v>0.85</v>
+        <v>0.73</v>
       </c>
       <c r="N8" s="4">
-        <v>0.63</v>
-      </c>
-      <c r="Q8" s="13"/>
-    </row>
-    <row r="9" spans="1:23">
-      <c r="A9" s="11" t="s">
+        <v>0.61</v>
+      </c>
+      <c r="Q8" s="11"/>
+    </row>
+    <row r="9" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="A9" s="9" t="s">
         <v>61</v>
       </c>
       <c r="B9" s="4">
         <v>0.89</v>
       </c>
-      <c r="C9" s="9">
+      <c r="C9" s="7">
         <v>62.1</v>
       </c>
-      <c r="D9" s="10">
+      <c r="D9" s="8">
         <v>6</v>
       </c>
-      <c r="E9" s="9">
+      <c r="E9" s="7">
         <v>75.099999999999994</v>
       </c>
-      <c r="F9" s="9">
+      <c r="F9" s="7">
         <v>82.8</v>
       </c>
-      <c r="G9" s="9">
+      <c r="G9" s="7">
         <v>90.3</v>
       </c>
       <c r="H9" s="4"/>
@@ -1212,32 +1250,32 @@
         <v>0.92</v>
       </c>
       <c r="M9" s="4">
-        <v>0.85</v>
+        <v>0.72</v>
       </c>
       <c r="N9" s="4">
-        <v>0.63</v>
-      </c>
-    </row>
-    <row r="10" spans="1:23">
-      <c r="A10" s="11" t="s">
+        <v>0.6</v>
+      </c>
+    </row>
+    <row r="10" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="A10" s="9" t="s">
         <v>47</v>
       </c>
       <c r="B10" s="4">
         <v>2.06</v>
       </c>
-      <c r="C10" s="9">
+      <c r="C10" s="7">
         <v>50</v>
       </c>
-      <c r="D10" s="10">
+      <c r="D10" s="8">
         <v>6</v>
       </c>
-      <c r="E10" s="9">
+      <c r="E10" s="7">
         <v>21.7</v>
       </c>
-      <c r="F10" s="9">
+      <c r="F10" s="7">
         <v>31.4</v>
       </c>
-      <c r="G10" s="9">
+      <c r="G10" s="7">
         <v>115.6</v>
       </c>
       <c r="H10" s="4"/>
@@ -1254,32 +1292,32 @@
         <v>0.21</v>
       </c>
       <c r="M10" s="4">
-        <v>0.72</v>
+        <v>0.55000000000000004</v>
       </c>
       <c r="N10" s="4">
-        <v>0.59</v>
-      </c>
-    </row>
-    <row r="11" spans="1:23">
-      <c r="A11" s="11" t="s">
+        <v>0.55000000000000004</v>
+      </c>
+    </row>
+    <row r="11" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="A11" s="9" t="s">
         <v>46</v>
       </c>
       <c r="B11" s="4">
         <v>1.52</v>
       </c>
-      <c r="C11" s="9">
+      <c r="C11" s="7">
         <v>48.1</v>
       </c>
-      <c r="D11" s="10">
+      <c r="D11" s="8">
         <v>5</v>
       </c>
-      <c r="E11" s="9">
+      <c r="E11" s="7">
         <v>25.3</v>
       </c>
-      <c r="F11" s="9">
+      <c r="F11" s="7">
         <v>46.6</v>
       </c>
-      <c r="G11" s="9">
+      <c r="G11" s="7">
         <v>105</v>
       </c>
       <c r="H11" s="4"/>
@@ -1296,116 +1334,116 @@
         <v>0.34</v>
       </c>
       <c r="M11" s="4">
-        <v>0.77</v>
+        <v>0.62</v>
       </c>
       <c r="N11" s="4">
-        <v>0.53</v>
-      </c>
-    </row>
-    <row r="12" spans="1:23">
-      <c r="A12" s="11" t="s">
-        <v>63</v>
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="12" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="A12" s="9" t="s">
+        <v>40</v>
       </c>
       <c r="B12" s="4">
-        <v>1.6</v>
-      </c>
-      <c r="C12" s="9">
-        <v>54.3</v>
-      </c>
-      <c r="D12" s="10">
+        <v>1.19</v>
+      </c>
+      <c r="C12" s="7">
+        <v>51.3</v>
+      </c>
+      <c r="D12" s="8">
         <v>5</v>
       </c>
-      <c r="E12" s="9">
-        <v>26.2</v>
-      </c>
-      <c r="F12" s="9">
-        <v>26.6</v>
-      </c>
-      <c r="G12" s="9">
-        <v>105.8</v>
+      <c r="E12" s="7">
+        <v>38.4</v>
+      </c>
+      <c r="F12" s="7">
+        <v>32</v>
+      </c>
+      <c r="G12" s="7">
+        <v>79.8</v>
       </c>
       <c r="H12" s="4"/>
       <c r="I12" s="4">
-        <v>0.69</v>
+        <v>0.42</v>
       </c>
       <c r="J12" s="4">
-        <v>0.51</v>
+        <v>0.47</v>
       </c>
       <c r="K12" s="4">
         <v>0.44</v>
       </c>
       <c r="L12" s="4">
-        <v>0.2</v>
+        <v>0.31</v>
       </c>
       <c r="M12" s="4">
-        <v>0.77</v>
+        <v>0.81</v>
       </c>
       <c r="N12" s="4">
-        <v>0.52</v>
-      </c>
-    </row>
-    <row r="13" spans="1:23">
-      <c r="A13" s="11" t="s">
-        <v>40</v>
+        <v>0.49</v>
+      </c>
+    </row>
+    <row r="13" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="A13" s="9" t="s">
+        <v>63</v>
       </c>
       <c r="B13" s="4">
-        <v>1.19</v>
-      </c>
-      <c r="C13" s="9">
-        <v>51.3</v>
-      </c>
-      <c r="D13" s="10">
+        <v>1.6</v>
+      </c>
+      <c r="C13" s="7">
+        <v>54.3</v>
+      </c>
+      <c r="D13" s="8">
         <v>5</v>
       </c>
-      <c r="E13" s="9">
-        <v>38.4</v>
-      </c>
-      <c r="F13" s="9">
-        <v>32</v>
-      </c>
-      <c r="G13" s="9">
-        <v>79.8</v>
+      <c r="E13" s="7">
+        <v>26.2</v>
+      </c>
+      <c r="F13" s="7">
+        <v>26.6</v>
+      </c>
+      <c r="G13" s="7">
+        <v>105.8</v>
       </c>
       <c r="H13" s="4"/>
       <c r="I13" s="4">
-        <v>0.42</v>
+        <v>0.69</v>
       </c>
       <c r="J13" s="4">
-        <v>0.47</v>
+        <v>0.51</v>
       </c>
       <c r="K13" s="4">
         <v>0.44</v>
       </c>
       <c r="L13" s="4">
-        <v>0.31</v>
+        <v>0.2</v>
       </c>
       <c r="M13" s="4">
-        <v>0.9</v>
+        <v>0.61</v>
       </c>
       <c r="N13" s="4">
-        <v>0.51</v>
-      </c>
-    </row>
-    <row r="14" spans="1:23">
-      <c r="A14" s="11" t="s">
+        <v>0.49</v>
+      </c>
+    </row>
+    <row r="14" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="A14" s="9" t="s">
         <v>41</v>
       </c>
       <c r="B14" s="4">
         <v>1.22</v>
       </c>
-      <c r="C14" s="9">
+      <c r="C14" s="7">
         <v>46.3</v>
       </c>
-      <c r="D14" s="10">
+      <c r="D14" s="8">
         <v>4</v>
       </c>
-      <c r="E14" s="9">
+      <c r="E14" s="7">
         <v>22.9</v>
       </c>
-      <c r="F14" s="9">
+      <c r="F14" s="7">
         <v>44.5</v>
       </c>
-      <c r="G14" s="9">
+      <c r="G14" s="7">
         <v>97.3</v>
       </c>
       <c r="H14" s="4"/>
@@ -1422,32 +1460,32 @@
         <v>0.31</v>
       </c>
       <c r="M14" s="4">
-        <v>0.81</v>
+        <v>0.67</v>
       </c>
       <c r="N14" s="4">
-        <v>0.46</v>
-      </c>
-    </row>
-    <row r="15" spans="1:23">
-      <c r="A15" s="11" t="s">
+        <v>0.43</v>
+      </c>
+    </row>
+    <row r="15" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="A15" s="9" t="s">
         <v>66</v>
       </c>
       <c r="B15" s="4">
         <v>0.89</v>
       </c>
-      <c r="C15" s="9">
+      <c r="C15" s="7">
         <v>51.2</v>
       </c>
-      <c r="D15" s="10">
+      <c r="D15" s="8">
         <v>5</v>
       </c>
-      <c r="E15" s="9">
+      <c r="E15" s="7">
         <v>42.4</v>
       </c>
-      <c r="F15" s="9">
+      <c r="F15" s="7">
         <v>45.7</v>
       </c>
-      <c r="G15" s="9">
+      <c r="G15" s="7">
         <v>113.2</v>
       </c>
       <c r="H15" s="4"/>
@@ -1464,284 +1502,284 @@
         <v>0.44</v>
       </c>
       <c r="M15" s="4">
-        <v>0.73</v>
+        <v>0.56999999999999995</v>
       </c>
       <c r="N15" s="4">
-        <v>0.46</v>
-      </c>
-    </row>
-    <row r="16" spans="1:23">
-      <c r="A16" s="11" t="s">
-        <v>45</v>
+        <v>0.43</v>
+      </c>
+    </row>
+    <row r="16" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="A16" s="9" t="s">
+        <v>42</v>
       </c>
       <c r="B16" s="4">
-        <v>1.1399999999999999</v>
-      </c>
-      <c r="C16" s="9">
-        <v>55.1</v>
-      </c>
-      <c r="D16" s="10">
-        <v>5</v>
-      </c>
-      <c r="E16" s="9">
-        <v>14.6</v>
-      </c>
-      <c r="F16" s="9">
-        <v>22.8</v>
-      </c>
-      <c r="G16" s="9">
-        <v>101.4</v>
+        <v>1.17</v>
+      </c>
+      <c r="C16" s="7">
+        <v>59.4</v>
+      </c>
+      <c r="D16" s="8">
+        <v>4</v>
+      </c>
+      <c r="E16" s="7">
+        <v>15.1</v>
+      </c>
+      <c r="F16" s="7">
+        <v>14.2</v>
+      </c>
+      <c r="G16" s="7">
+        <v>88.9</v>
       </c>
       <c r="H16" s="4"/>
       <c r="I16" s="4">
-        <v>0.39</v>
+        <v>0.41</v>
       </c>
       <c r="J16" s="4">
-        <v>0.52</v>
+        <v>0.56999999999999995</v>
       </c>
       <c r="K16" s="4">
-        <v>0.44</v>
+        <v>0.33</v>
       </c>
       <c r="L16" s="4">
-        <v>0.1</v>
+        <v>0.03</v>
       </c>
       <c r="M16" s="4">
-        <v>0.79</v>
+        <v>0.74</v>
       </c>
       <c r="N16" s="4">
-        <v>0.45</v>
-      </c>
-    </row>
-    <row r="17" spans="1:14">
-      <c r="A17" s="11" t="s">
-        <v>42</v>
+        <v>0.42</v>
+      </c>
+    </row>
+    <row r="17" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A17" s="9" t="s">
+        <v>45</v>
       </c>
       <c r="B17" s="4">
-        <v>1.17</v>
-      </c>
-      <c r="C17" s="9">
-        <v>59.4</v>
-      </c>
-      <c r="D17" s="10">
-        <v>4</v>
-      </c>
-      <c r="E17" s="9">
-        <v>15.1</v>
-      </c>
-      <c r="F17" s="9">
-        <v>14.2</v>
-      </c>
-      <c r="G17" s="9">
-        <v>88.9</v>
+        <v>1.1399999999999999</v>
+      </c>
+      <c r="C17" s="7">
+        <v>55.1</v>
+      </c>
+      <c r="D17" s="8">
+        <v>5</v>
+      </c>
+      <c r="E17" s="7">
+        <v>14.6</v>
+      </c>
+      <c r="F17" s="7">
+        <v>22.8</v>
+      </c>
+      <c r="G17" s="7">
+        <v>101.4</v>
       </c>
       <c r="H17" s="4"/>
       <c r="I17" s="4">
-        <v>0.41</v>
+        <v>0.39</v>
       </c>
       <c r="J17" s="4">
-        <v>0.56999999999999995</v>
+        <v>0.52</v>
       </c>
       <c r="K17" s="4">
-        <v>0.33</v>
+        <v>0.44</v>
       </c>
       <c r="L17" s="4">
-        <v>0.03</v>
+        <v>0.1</v>
       </c>
       <c r="M17" s="4">
-        <v>0.86</v>
+        <v>0.64</v>
       </c>
       <c r="N17" s="4">
-        <v>0.44</v>
-      </c>
-    </row>
-    <row r="18" spans="1:14">
-      <c r="A18" s="11" t="s">
-        <v>44</v>
+        <v>0.42</v>
+      </c>
+    </row>
+    <row r="18" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A18" s="9" t="s">
+        <v>67</v>
       </c>
       <c r="B18" s="4">
-        <v>0.99</v>
-      </c>
-      <c r="C18" s="9">
-        <v>46.8</v>
-      </c>
-      <c r="D18" s="10">
-        <v>5</v>
-      </c>
-      <c r="E18" s="9">
-        <v>18</v>
-      </c>
-      <c r="F18" s="9">
-        <v>32.1</v>
-      </c>
-      <c r="G18" s="9">
-        <v>101.7</v>
+        <v>1.02</v>
+      </c>
+      <c r="C18" s="7">
+        <v>48.1</v>
+      </c>
+      <c r="D18" s="8">
+        <v>4</v>
+      </c>
+      <c r="E18" s="7">
+        <v>24.6</v>
+      </c>
+      <c r="F18" s="7">
+        <v>18.8</v>
+      </c>
+      <c r="G18" s="7">
+        <v>68.400000000000006</v>
       </c>
       <c r="H18" s="4"/>
       <c r="I18" s="4">
-        <v>0.28999999999999998</v>
+        <v>0.31</v>
       </c>
       <c r="J18" s="4">
+        <v>0.44</v>
+      </c>
+      <c r="K18" s="4">
+        <v>0.33</v>
+      </c>
+      <c r="L18" s="4">
+        <v>0.13</v>
+      </c>
+      <c r="M18" s="4">
+        <v>0.92</v>
+      </c>
+      <c r="N18" s="4">
         <v>0.42</v>
       </c>
-      <c r="K18" s="4">
-        <v>0.44</v>
-      </c>
-      <c r="L18" s="4">
-        <v>0.19</v>
-      </c>
-      <c r="M18" s="4">
-        <v>0.79</v>
-      </c>
-      <c r="N18" s="4">
-        <v>0.43</v>
-      </c>
-    </row>
-    <row r="19" spans="1:14">
-      <c r="A19" s="11" t="s">
-        <v>67</v>
+    </row>
+    <row r="19" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A19" s="9" t="s">
+        <v>44</v>
       </c>
       <c r="B19" s="4">
-        <v>1.02</v>
-      </c>
-      <c r="C19" s="9">
-        <v>48.1</v>
-      </c>
-      <c r="D19" s="10">
-        <v>4</v>
-      </c>
-      <c r="E19" s="9">
-        <v>24.6</v>
-      </c>
-      <c r="F19" s="9">
-        <v>18.8</v>
-      </c>
-      <c r="G19" s="9">
-        <v>68.400000000000006</v>
+        <v>0.99</v>
+      </c>
+      <c r="C19" s="7">
+        <v>46.8</v>
+      </c>
+      <c r="D19" s="8">
+        <v>5</v>
+      </c>
+      <c r="E19" s="7">
+        <v>18</v>
+      </c>
+      <c r="F19" s="7">
+        <v>32.1</v>
+      </c>
+      <c r="G19" s="7">
+        <v>101.7</v>
       </c>
       <c r="H19" s="4"/>
       <c r="I19" s="4">
-        <v>0.31</v>
+        <v>0.28999999999999998</v>
       </c>
       <c r="J19" s="4">
+        <v>0.42</v>
+      </c>
+      <c r="K19" s="4">
         <v>0.44</v>
       </c>
-      <c r="K19" s="4">
-        <v>0.33</v>
-      </c>
       <c r="L19" s="4">
-        <v>0.13</v>
+        <v>0.19</v>
       </c>
       <c r="M19" s="4">
-        <v>0.96</v>
+        <v>0.64</v>
       </c>
       <c r="N19" s="4">
-        <v>0.43</v>
-      </c>
-    </row>
-    <row r="20" spans="1:14">
-      <c r="A20" s="11" t="s">
-        <v>48</v>
+        <v>0.4</v>
+      </c>
+    </row>
+    <row r="20" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A20" s="9" t="s">
+        <v>56</v>
       </c>
       <c r="B20" s="4">
-        <v>0.56000000000000005</v>
-      </c>
-      <c r="C20" s="9">
-        <v>35.4</v>
-      </c>
-      <c r="D20" s="10">
-        <v>6</v>
-      </c>
-      <c r="E20" s="9">
-        <v>48</v>
-      </c>
-      <c r="F20" s="9">
-        <v>65.7</v>
-      </c>
-      <c r="G20" s="9">
-        <v>134.1</v>
+        <v>0.71</v>
+      </c>
+      <c r="C20" s="7">
+        <v>26.1</v>
+      </c>
+      <c r="D20" s="8">
+        <v>3</v>
+      </c>
+      <c r="E20" s="7">
+        <v>58.1</v>
+      </c>
+      <c r="F20" s="7">
+        <v>79.900000000000006</v>
+      </c>
+      <c r="G20" s="7">
+        <v>101.2</v>
       </c>
       <c r="H20" s="4"/>
       <c r="I20" s="4">
-        <v>0</v>
+        <v>0.1</v>
       </c>
       <c r="J20" s="4">
-        <v>0.28999999999999998</v>
+        <v>0.17</v>
       </c>
       <c r="K20" s="4">
+        <v>0.22</v>
+      </c>
+      <c r="L20" s="4">
+        <v>0.79</v>
+      </c>
+      <c r="M20" s="4">
+        <v>0.64</v>
+      </c>
+      <c r="N20" s="4">
+        <v>0.39</v>
+      </c>
+    </row>
+    <row r="21" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A21" s="9" t="s">
+        <v>48</v>
+      </c>
+      <c r="B21" s="4">
         <v>0.56000000000000005</v>
       </c>
-      <c r="L20" s="4">
-        <v>0.63</v>
-      </c>
-      <c r="M20" s="4">
-        <v>0.62</v>
-      </c>
-      <c r="N20" s="4">
-        <v>0.42</v>
-      </c>
-    </row>
-    <row r="21" spans="1:14">
-      <c r="A21" s="11" t="s">
-        <v>56</v>
-      </c>
-      <c r="B21" s="4">
-        <v>0.71</v>
-      </c>
-      <c r="C21" s="9">
-        <v>26.1</v>
-      </c>
-      <c r="D21" s="10">
-        <v>3</v>
-      </c>
-      <c r="E21" s="9">
-        <v>58.1</v>
-      </c>
-      <c r="F21" s="9">
-        <v>79.900000000000006</v>
-      </c>
-      <c r="G21" s="9">
-        <v>101.2</v>
+      <c r="C21" s="7">
+        <v>35.4</v>
+      </c>
+      <c r="D21" s="8">
+        <v>6</v>
+      </c>
+      <c r="E21" s="7">
+        <v>48</v>
+      </c>
+      <c r="F21" s="7">
+        <v>65.7</v>
+      </c>
+      <c r="G21" s="7">
+        <v>134.1</v>
       </c>
       <c r="H21" s="4"/>
       <c r="I21" s="4">
-        <v>0.1</v>
+        <v>0</v>
       </c>
       <c r="J21" s="4">
-        <v>0.17</v>
+        <v>0.28999999999999998</v>
       </c>
       <c r="K21" s="4">
-        <v>0.22</v>
+        <v>0.56000000000000005</v>
       </c>
       <c r="L21" s="4">
-        <v>0.79</v>
+        <v>0.63</v>
       </c>
       <c r="M21" s="4">
-        <v>0.79</v>
+        <v>0.45</v>
       </c>
       <c r="N21" s="4">
-        <v>0.42</v>
-      </c>
-    </row>
-    <row r="22" spans="1:14">
-      <c r="A22" s="11" t="s">
+        <v>0.38</v>
+      </c>
+    </row>
+    <row r="22" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A22" s="9" t="s">
         <v>68</v>
       </c>
       <c r="B22" s="4">
         <v>1.02</v>
       </c>
-      <c r="C22" s="9">
+      <c r="C22" s="7">
         <v>25</v>
       </c>
-      <c r="D22" s="10">
+      <c r="D22" s="8">
         <v>5</v>
       </c>
-      <c r="E22" s="9">
+      <c r="E22" s="7">
         <v>15.4</v>
       </c>
-      <c r="F22" s="9">
+      <c r="F22" s="7">
         <v>27.9</v>
       </c>
-      <c r="G22" s="9">
+      <c r="G22" s="7">
         <v>118</v>
       </c>
       <c r="H22" s="4"/>
@@ -1758,32 +1796,32 @@
         <v>0.14000000000000001</v>
       </c>
       <c r="M22" s="4">
-        <v>0.7</v>
+        <v>0.54</v>
       </c>
       <c r="N22" s="4">
-        <v>0.35</v>
-      </c>
-    </row>
-    <row r="23" spans="1:14">
-      <c r="A23" s="11" t="s">
+        <v>0.32</v>
+      </c>
+    </row>
+    <row r="23" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A23" s="9" t="s">
         <v>43</v>
       </c>
       <c r="B23" s="4">
         <v>1.04</v>
       </c>
-      <c r="C23" s="9">
+      <c r="C23" s="7">
         <v>27.4</v>
       </c>
-      <c r="D23" s="10">
+      <c r="D23" s="8">
         <v>2</v>
       </c>
-      <c r="E23" s="9">
+      <c r="E23" s="7">
         <v>16.7</v>
       </c>
-      <c r="F23" s="9">
+      <c r="F23" s="7">
         <v>25.6</v>
       </c>
-      <c r="G23" s="9">
+      <c r="G23" s="7">
         <v>79.8</v>
       </c>
       <c r="H23" s="4"/>
@@ -1800,116 +1838,116 @@
         <v>0.13</v>
       </c>
       <c r="M23" s="4">
-        <v>0.9</v>
+        <v>0.81</v>
       </c>
       <c r="N23" s="4">
-        <v>0.33</v>
-      </c>
-    </row>
-    <row r="24" spans="1:14">
-      <c r="A24" s="11" t="s">
-        <v>58</v>
+        <v>0.31</v>
+      </c>
+    </row>
+    <row r="24" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A24" s="9" t="s">
+        <v>54</v>
       </c>
       <c r="B24" s="4">
-        <v>0.76</v>
-      </c>
-      <c r="C24" s="9">
-        <v>17.100000000000001</v>
-      </c>
-      <c r="D24" s="10">
+        <v>0.69</v>
+      </c>
+      <c r="C24" s="7">
+        <v>27.1</v>
+      </c>
+      <c r="D24" s="8">
         <v>2</v>
       </c>
-      <c r="E24" s="9">
-        <v>55.3</v>
-      </c>
-      <c r="F24" s="9">
-        <v>71.7</v>
-      </c>
-      <c r="G24" s="9">
-        <v>154.6</v>
+      <c r="E24" s="7">
+        <v>10</v>
+      </c>
+      <c r="F24" s="7">
+        <v>13.7</v>
+      </c>
+      <c r="G24" s="7">
+        <v>60.9</v>
       </c>
       <c r="H24" s="4"/>
       <c r="I24" s="4">
-        <v>0.14000000000000001</v>
+        <v>0.08</v>
       </c>
       <c r="J24" s="4">
-        <v>7.0000000000000007E-2</v>
+        <v>0.19</v>
       </c>
       <c r="K24" s="4">
         <v>0.11</v>
       </c>
       <c r="L24" s="4">
-        <v>0.71</v>
+        <v>0</v>
       </c>
       <c r="M24" s="4">
-        <v>0.51</v>
+        <v>1</v>
       </c>
       <c r="N24" s="4">
-        <v>0.31</v>
-      </c>
-    </row>
-    <row r="25" spans="1:14">
-      <c r="A25" s="11" t="s">
-        <v>52</v>
+        <v>0.28000000000000003</v>
+      </c>
+    </row>
+    <row r="25" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A25" s="9" t="s">
+        <v>58</v>
       </c>
       <c r="B25" s="4">
-        <v>0.91</v>
-      </c>
-      <c r="C25" s="9">
-        <v>37.200000000000003</v>
-      </c>
-      <c r="D25" s="10">
+        <v>0.76</v>
+      </c>
+      <c r="C25" s="7">
+        <v>17.100000000000001</v>
+      </c>
+      <c r="D25" s="8">
         <v>2</v>
       </c>
-      <c r="E25" s="9">
-        <v>17.100000000000001</v>
-      </c>
-      <c r="F25" s="9">
-        <v>28.7</v>
-      </c>
-      <c r="G25" s="9">
-        <v>122.9</v>
+      <c r="E25" s="7">
+        <v>55.3</v>
+      </c>
+      <c r="F25" s="7">
+        <v>71.7</v>
+      </c>
+      <c r="G25" s="7">
+        <v>154.6</v>
       </c>
       <c r="H25" s="4"/>
       <c r="I25" s="4">
-        <v>0.24</v>
+        <v>0.14000000000000001</v>
       </c>
       <c r="J25" s="4">
-        <v>0.31</v>
+        <v>7.0000000000000007E-2</v>
       </c>
       <c r="K25" s="4">
         <v>0.11</v>
       </c>
       <c r="L25" s="4">
-        <v>0.16</v>
+        <v>0.71</v>
       </c>
       <c r="M25" s="4">
-        <v>0.68</v>
+        <v>0.35</v>
       </c>
       <c r="N25" s="4">
-        <v>0.3</v>
-      </c>
-    </row>
-    <row r="26" spans="1:14">
-      <c r="A26" s="11" t="s">
+        <v>0.28000000000000003</v>
+      </c>
+    </row>
+    <row r="26" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A26" s="9" t="s">
         <v>50</v>
       </c>
       <c r="B26" s="4">
         <v>0.84</v>
       </c>
-      <c r="C26" s="9">
+      <c r="C26" s="7">
         <v>11.6</v>
       </c>
-      <c r="D26" s="10">
+      <c r="D26" s="8">
         <v>2</v>
       </c>
-      <c r="E26" s="9">
+      <c r="E26" s="7">
         <v>32.4</v>
       </c>
-      <c r="F26" s="9">
+      <c r="F26" s="7">
         <v>55.3</v>
       </c>
-      <c r="G26" s="9">
+      <c r="G26" s="7">
         <v>117.9</v>
       </c>
       <c r="H26" s="4"/>
@@ -1926,74 +1964,74 @@
         <v>0.45</v>
       </c>
       <c r="M26" s="4">
-        <v>0.7</v>
+        <v>0.54</v>
       </c>
       <c r="N26" s="4">
-        <v>0.28999999999999998</v>
-      </c>
-    </row>
-    <row r="27" spans="1:14">
-      <c r="A27" s="11" t="s">
-        <v>54</v>
+        <v>0.26</v>
+      </c>
+    </row>
+    <row r="27" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A27" s="9" t="s">
+        <v>52</v>
       </c>
       <c r="B27" s="4">
-        <v>0.69</v>
-      </c>
-      <c r="C27" s="9">
-        <v>27.1</v>
-      </c>
-      <c r="D27" s="10">
+        <v>0.91</v>
+      </c>
+      <c r="C27" s="7">
+        <v>37.200000000000003</v>
+      </c>
+      <c r="D27" s="8">
         <v>2</v>
       </c>
-      <c r="E27" s="9">
-        <v>10</v>
-      </c>
-      <c r="F27" s="9">
-        <v>13.7</v>
-      </c>
-      <c r="G27" s="9">
-        <v>60.9</v>
+      <c r="E27" s="7">
+        <v>17.100000000000001</v>
+      </c>
+      <c r="F27" s="7">
+        <v>28.7</v>
+      </c>
+      <c r="G27" s="7">
+        <v>122.9</v>
       </c>
       <c r="H27" s="4"/>
       <c r="I27" s="4">
-        <v>0.08</v>
+        <v>0.24</v>
       </c>
       <c r="J27" s="4">
-        <v>0.19</v>
+        <v>0.31</v>
       </c>
       <c r="K27" s="4">
         <v>0.11</v>
       </c>
       <c r="L27" s="4">
-        <v>0</v>
+        <v>0.16</v>
       </c>
       <c r="M27" s="4">
-        <v>1</v>
+        <v>0.51</v>
       </c>
       <c r="N27" s="4">
-        <v>0.28000000000000003</v>
-      </c>
-    </row>
-    <row r="28" spans="1:14">
-      <c r="A28" s="11" t="s">
+        <v>0.26</v>
+      </c>
+    </row>
+    <row r="28" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A28" s="9" t="s">
         <v>49</v>
       </c>
       <c r="B28" s="4">
         <v>0.64</v>
       </c>
-      <c r="C28" s="9">
+      <c r="C28" s="7">
         <v>15.9</v>
       </c>
-      <c r="D28" s="10">
+      <c r="D28" s="8">
         <v>2</v>
       </c>
-      <c r="E28" s="9">
+      <c r="E28" s="7">
         <v>25.7</v>
       </c>
-      <c r="F28" s="9">
+      <c r="F28" s="7">
         <v>47.9</v>
       </c>
-      <c r="G28" s="9">
+      <c r="G28" s="7">
         <v>107.7</v>
       </c>
       <c r="H28" s="4"/>
@@ -2010,32 +2048,32 @@
         <v>0.36</v>
       </c>
       <c r="M28" s="4">
-        <v>0.76</v>
+        <v>0.6</v>
       </c>
       <c r="N28" s="4">
-        <v>0.27</v>
-      </c>
-    </row>
-    <row r="29" spans="1:14">
-      <c r="A29" s="11" t="s">
+        <v>0.23</v>
+      </c>
+    </row>
+    <row r="29" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A29" s="9" t="s">
         <v>55</v>
       </c>
       <c r="B29" s="4">
         <v>0.76</v>
       </c>
-      <c r="C29" s="9">
+      <c r="C29" s="7">
         <v>17.600000000000001</v>
       </c>
-      <c r="D29" s="10">
+      <c r="D29" s="8">
         <v>1</v>
       </c>
-      <c r="E29" s="9">
+      <c r="E29" s="7">
         <v>48.4</v>
       </c>
-      <c r="F29" s="9">
+      <c r="F29" s="7">
         <v>63.4</v>
       </c>
-      <c r="G29" s="9">
+      <c r="G29" s="7">
         <v>182.9</v>
       </c>
       <c r="H29" s="4"/>
@@ -2052,32 +2090,32 @@
         <v>0.61</v>
       </c>
       <c r="M29" s="4">
-        <v>0.37</v>
+        <v>0.23</v>
       </c>
       <c r="N29" s="4">
-        <v>0.24</v>
-      </c>
-    </row>
-    <row r="30" spans="1:14">
-      <c r="A30" s="11" t="s">
+        <v>0.21</v>
+      </c>
+    </row>
+    <row r="30" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A30" s="9" t="s">
         <v>53</v>
       </c>
       <c r="B30" s="4">
         <v>0.64</v>
       </c>
-      <c r="C30" s="9">
+      <c r="C30" s="7">
         <v>16.3</v>
       </c>
-      <c r="D30" s="10">
+      <c r="D30" s="8">
         <v>2</v>
       </c>
-      <c r="E30" s="9">
+      <c r="E30" s="7">
         <v>16</v>
       </c>
-      <c r="F30" s="9">
+      <c r="F30" s="7">
         <v>29.1</v>
       </c>
-      <c r="G30" s="9">
+      <c r="G30" s="7">
         <v>102.3</v>
       </c>
       <c r="H30" s="4"/>
@@ -2094,32 +2132,32 @@
         <v>0.15</v>
       </c>
       <c r="M30" s="4">
-        <v>0.79</v>
+        <v>0.64</v>
       </c>
       <c r="N30" s="4">
-        <v>0.23</v>
-      </c>
-    </row>
-    <row r="31" spans="1:14">
-      <c r="A31" s="11" t="s">
+        <v>0.2</v>
+      </c>
+    </row>
+    <row r="31" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A31" s="9" t="s">
         <v>57</v>
       </c>
       <c r="B31" s="4">
         <v>0.81</v>
       </c>
-      <c r="C31" s="9">
+      <c r="C31" s="7">
         <v>13.5</v>
       </c>
-      <c r="D31" s="10">
+      <c r="D31" s="8">
         <v>1</v>
       </c>
-      <c r="E31" s="9">
+      <c r="E31" s="7">
         <v>40</v>
       </c>
-      <c r="F31" s="9">
+      <c r="F31" s="7">
         <v>62.2</v>
       </c>
-      <c r="G31" s="9">
+      <c r="G31" s="7">
         <v>253.9</v>
       </c>
       <c r="H31" s="4"/>
@@ -2161,6 +2199,1329 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B8F3AC94-5516-B143-92CD-79450C18DEC4}">
+  <dimension ref="A1:W31"/>
+  <sheetViews>
+    <sheetView showRuler="0" workbookViewId="0">
+      <selection activeCell="A3" sqref="A3:B31"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="21.33203125" customWidth="1"/>
+    <col min="2" max="2" width="7.83203125" customWidth="1"/>
+    <col min="3" max="3" width="7" customWidth="1"/>
+    <col min="4" max="4" width="7.1640625" customWidth="1"/>
+    <col min="5" max="5" width="7" customWidth="1"/>
+    <col min="6" max="6" width="8.1640625" customWidth="1"/>
+    <col min="7" max="7" width="7.6640625" customWidth="1"/>
+    <col min="8" max="8" width="1.6640625" customWidth="1"/>
+    <col min="9" max="9" width="7.83203125" customWidth="1"/>
+    <col min="10" max="10" width="6.1640625" customWidth="1"/>
+    <col min="11" max="11" width="6.6640625" customWidth="1"/>
+    <col min="12" max="13" width="7.6640625" customWidth="1"/>
+    <col min="14" max="14" width="5.33203125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:23" ht="17" x14ac:dyDescent="0.25">
+      <c r="A1" s="1"/>
+      <c r="B1" s="17" t="s">
+        <v>71</v>
+      </c>
+      <c r="C1" s="18"/>
+      <c r="D1" s="18"/>
+      <c r="E1" s="18"/>
+      <c r="F1" s="18"/>
+      <c r="G1" s="18"/>
+      <c r="H1" s="5"/>
+      <c r="I1" s="15" t="s">
+        <v>36</v>
+      </c>
+      <c r="J1" s="15"/>
+      <c r="K1" s="15"/>
+      <c r="L1" s="15"/>
+      <c r="M1" s="16"/>
+      <c r="N1" s="1"/>
+    </row>
+    <row r="2" spans="1:23" ht="33" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A2" s="2" t="s">
+        <v>70</v>
+      </c>
+      <c r="B2" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="C2" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="D2" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="E2" s="3" t="s">
+        <v>69</v>
+      </c>
+      <c r="F2" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="G2" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="H2" s="3"/>
+      <c r="I2" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="J2" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="K2" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="L2" s="14" t="s">
+        <v>72</v>
+      </c>
+      <c r="M2" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="N2" s="6" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="3" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="A3" s="9" t="s">
+        <v>64</v>
+      </c>
+      <c r="B3" s="4">
+        <v>2.06</v>
+      </c>
+      <c r="C3" s="7">
+        <v>95.2</v>
+      </c>
+      <c r="D3" s="8">
+        <v>5</v>
+      </c>
+      <c r="E3" s="7">
+        <v>59.4</v>
+      </c>
+      <c r="F3" s="7">
+        <v>86.1</v>
+      </c>
+      <c r="G3" s="7">
+        <v>73.400000000000006</v>
+      </c>
+      <c r="H3" s="4"/>
+      <c r="I3" s="4">
+        <v>1</v>
+      </c>
+      <c r="J3" s="4">
+        <v>1</v>
+      </c>
+      <c r="K3" s="4">
+        <v>0.44</v>
+      </c>
+      <c r="L3" s="4">
+        <v>0.85</v>
+      </c>
+      <c r="M3" s="4">
+        <v>0.94</v>
+      </c>
+      <c r="N3" s="4">
+        <v>0.85</v>
+      </c>
+    </row>
+    <row r="4" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="A4" s="9" t="s">
+        <v>59</v>
+      </c>
+      <c r="B4" s="4">
+        <v>1.73</v>
+      </c>
+      <c r="C4" s="7">
+        <v>51.4</v>
+      </c>
+      <c r="D4" s="8">
+        <v>10</v>
+      </c>
+      <c r="E4" s="7">
+        <v>67.3</v>
+      </c>
+      <c r="F4" s="7">
+        <v>90</v>
+      </c>
+      <c r="G4" s="7">
+        <v>79.2</v>
+      </c>
+      <c r="H4" s="4"/>
+      <c r="I4" s="4">
+        <v>0.78</v>
+      </c>
+      <c r="J4" s="4">
+        <v>0.48</v>
+      </c>
+      <c r="K4" s="4">
+        <v>1</v>
+      </c>
+      <c r="L4" s="4">
+        <v>0.93</v>
+      </c>
+      <c r="M4" s="4">
+        <v>0.91</v>
+      </c>
+      <c r="N4" s="4">
+        <v>0.82</v>
+      </c>
+    </row>
+    <row r="5" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="A5" s="9" t="s">
+        <v>62</v>
+      </c>
+      <c r="B5" s="4">
+        <v>1.6</v>
+      </c>
+      <c r="C5" s="7">
+        <v>41.2</v>
+      </c>
+      <c r="D5" s="8">
+        <v>10</v>
+      </c>
+      <c r="E5" s="7">
+        <v>77</v>
+      </c>
+      <c r="F5" s="7">
+        <v>92</v>
+      </c>
+      <c r="G5" s="7">
+        <v>79.7</v>
+      </c>
+      <c r="H5" s="4"/>
+      <c r="I5" s="4">
+        <v>0.69</v>
+      </c>
+      <c r="J5" s="4">
+        <v>0.35</v>
+      </c>
+      <c r="K5" s="4">
+        <v>1</v>
+      </c>
+      <c r="L5" s="4">
+        <v>1</v>
+      </c>
+      <c r="M5" s="4">
+        <v>0.9</v>
+      </c>
+      <c r="N5" s="4">
+        <v>0.79</v>
+      </c>
+    </row>
+    <row r="6" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="A6" s="9" t="s">
+        <v>65</v>
+      </c>
+      <c r="B6" s="4">
+        <v>2.06</v>
+      </c>
+      <c r="C6" s="7">
+        <v>85.6</v>
+      </c>
+      <c r="D6" s="8">
+        <v>8</v>
+      </c>
+      <c r="E6" s="7">
+        <v>42.6</v>
+      </c>
+      <c r="F6" s="7">
+        <v>75.8</v>
+      </c>
+      <c r="G6" s="7">
+        <v>148.5</v>
+      </c>
+      <c r="H6" s="4"/>
+      <c r="I6" s="4">
+        <v>1</v>
+      </c>
+      <c r="J6" s="4">
+        <v>0.89</v>
+      </c>
+      <c r="K6" s="4">
+        <v>0.78</v>
+      </c>
+      <c r="L6" s="4">
+        <v>0.67</v>
+      </c>
+      <c r="M6" s="4">
+        <v>0.55000000000000004</v>
+      </c>
+      <c r="N6" s="4">
+        <v>0.78</v>
+      </c>
+      <c r="Q6" s="10"/>
+    </row>
+    <row r="7" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="A7" s="9" t="s">
+        <v>60</v>
+      </c>
+      <c r="B7" s="4">
+        <v>1.83</v>
+      </c>
+      <c r="C7" s="7">
+        <v>62.3</v>
+      </c>
+      <c r="D7" s="8">
+        <v>10</v>
+      </c>
+      <c r="E7" s="7">
+        <v>55.6</v>
+      </c>
+      <c r="F7" s="7">
+        <v>77.099999999999994</v>
+      </c>
+      <c r="G7" s="7">
+        <v>128.5</v>
+      </c>
+      <c r="H7" s="4"/>
+      <c r="I7" s="4">
+        <v>0.85</v>
+      </c>
+      <c r="J7" s="4">
+        <v>0.61</v>
+      </c>
+      <c r="K7" s="4">
+        <v>1</v>
+      </c>
+      <c r="L7" s="4">
+        <v>0.76</v>
+      </c>
+      <c r="M7" s="4">
+        <v>0.65</v>
+      </c>
+      <c r="N7" s="4">
+        <v>0.77</v>
+      </c>
+      <c r="R7" s="12"/>
+      <c r="S7" s="13"/>
+      <c r="T7" s="13"/>
+      <c r="U7" s="13"/>
+      <c r="V7" s="13"/>
+      <c r="W7" s="13"/>
+    </row>
+    <row r="8" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="A8" s="9" t="s">
+        <v>51</v>
+      </c>
+      <c r="B8" s="4">
+        <v>1.6</v>
+      </c>
+      <c r="C8" s="7">
+        <v>51.1</v>
+      </c>
+      <c r="D8" s="8">
+        <v>9</v>
+      </c>
+      <c r="E8" s="7">
+        <v>27.9</v>
+      </c>
+      <c r="F8" s="7">
+        <v>34.6</v>
+      </c>
+      <c r="G8" s="7">
+        <v>89.9</v>
+      </c>
+      <c r="H8" s="4"/>
+      <c r="I8" s="4">
+        <v>0.69</v>
+      </c>
+      <c r="J8" s="4">
+        <v>0.47</v>
+      </c>
+      <c r="K8" s="4">
+        <v>0.89</v>
+      </c>
+      <c r="L8" s="4">
+        <v>0.27</v>
+      </c>
+      <c r="M8" s="4">
+        <v>0.85</v>
+      </c>
+      <c r="N8" s="4">
+        <v>0.63</v>
+      </c>
+      <c r="Q8" s="11"/>
+    </row>
+    <row r="9" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="A9" s="9" t="s">
+        <v>61</v>
+      </c>
+      <c r="B9" s="4">
+        <v>0.89</v>
+      </c>
+      <c r="C9" s="7">
+        <v>62.1</v>
+      </c>
+      <c r="D9" s="8">
+        <v>6</v>
+      </c>
+      <c r="E9" s="7">
+        <v>75.099999999999994</v>
+      </c>
+      <c r="F9" s="7">
+        <v>82.8</v>
+      </c>
+      <c r="G9" s="7">
+        <v>90.3</v>
+      </c>
+      <c r="H9" s="4"/>
+      <c r="I9" s="4">
+        <v>0.22</v>
+      </c>
+      <c r="J9" s="4">
+        <v>0.6</v>
+      </c>
+      <c r="K9" s="4">
+        <v>0.56000000000000005</v>
+      </c>
+      <c r="L9" s="4">
+        <v>0.92</v>
+      </c>
+      <c r="M9" s="4">
+        <v>0.85</v>
+      </c>
+      <c r="N9" s="4">
+        <v>0.63</v>
+      </c>
+    </row>
+    <row r="10" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="A10" s="9" t="s">
+        <v>47</v>
+      </c>
+      <c r="B10" s="4">
+        <v>2.06</v>
+      </c>
+      <c r="C10" s="7">
+        <v>50</v>
+      </c>
+      <c r="D10" s="8">
+        <v>6</v>
+      </c>
+      <c r="E10" s="7">
+        <v>21.7</v>
+      </c>
+      <c r="F10" s="7">
+        <v>31.4</v>
+      </c>
+      <c r="G10" s="7">
+        <v>115.6</v>
+      </c>
+      <c r="H10" s="4"/>
+      <c r="I10" s="4">
+        <v>1</v>
+      </c>
+      <c r="J10" s="4">
+        <v>0.46</v>
+      </c>
+      <c r="K10" s="4">
+        <v>0.56000000000000005</v>
+      </c>
+      <c r="L10" s="4">
+        <v>0.21</v>
+      </c>
+      <c r="M10" s="4">
+        <v>0.72</v>
+      </c>
+      <c r="N10" s="4">
+        <v>0.59</v>
+      </c>
+    </row>
+    <row r="11" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="A11" s="9" t="s">
+        <v>46</v>
+      </c>
+      <c r="B11" s="4">
+        <v>1.52</v>
+      </c>
+      <c r="C11" s="7">
+        <v>48.1</v>
+      </c>
+      <c r="D11" s="8">
+        <v>5</v>
+      </c>
+      <c r="E11" s="7">
+        <v>25.3</v>
+      </c>
+      <c r="F11" s="7">
+        <v>46.6</v>
+      </c>
+      <c r="G11" s="7">
+        <v>105</v>
+      </c>
+      <c r="H11" s="4"/>
+      <c r="I11" s="4">
+        <v>0.64</v>
+      </c>
+      <c r="J11" s="4">
+        <v>0.44</v>
+      </c>
+      <c r="K11" s="4">
+        <v>0.44</v>
+      </c>
+      <c r="L11" s="4">
+        <v>0.34</v>
+      </c>
+      <c r="M11" s="4">
+        <v>0.77</v>
+      </c>
+      <c r="N11" s="4">
+        <v>0.53</v>
+      </c>
+    </row>
+    <row r="12" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="A12" s="9" t="s">
+        <v>63</v>
+      </c>
+      <c r="B12" s="4">
+        <v>1.6</v>
+      </c>
+      <c r="C12" s="7">
+        <v>54.3</v>
+      </c>
+      <c r="D12" s="8">
+        <v>5</v>
+      </c>
+      <c r="E12" s="7">
+        <v>26.2</v>
+      </c>
+      <c r="F12" s="7">
+        <v>26.6</v>
+      </c>
+      <c r="G12" s="7">
+        <v>105.8</v>
+      </c>
+      <c r="H12" s="4"/>
+      <c r="I12" s="4">
+        <v>0.69</v>
+      </c>
+      <c r="J12" s="4">
+        <v>0.51</v>
+      </c>
+      <c r="K12" s="4">
+        <v>0.44</v>
+      </c>
+      <c r="L12" s="4">
+        <v>0.2</v>
+      </c>
+      <c r="M12" s="4">
+        <v>0.77</v>
+      </c>
+      <c r="N12" s="4">
+        <v>0.52</v>
+      </c>
+    </row>
+    <row r="13" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="A13" s="9" t="s">
+        <v>40</v>
+      </c>
+      <c r="B13" s="4">
+        <v>1.19</v>
+      </c>
+      <c r="C13" s="7">
+        <v>51.3</v>
+      </c>
+      <c r="D13" s="8">
+        <v>5</v>
+      </c>
+      <c r="E13" s="7">
+        <v>38.4</v>
+      </c>
+      <c r="F13" s="7">
+        <v>32</v>
+      </c>
+      <c r="G13" s="7">
+        <v>79.8</v>
+      </c>
+      <c r="H13" s="4"/>
+      <c r="I13" s="4">
+        <v>0.42</v>
+      </c>
+      <c r="J13" s="4">
+        <v>0.47</v>
+      </c>
+      <c r="K13" s="4">
+        <v>0.44</v>
+      </c>
+      <c r="L13" s="4">
+        <v>0.31</v>
+      </c>
+      <c r="M13" s="4">
+        <v>0.9</v>
+      </c>
+      <c r="N13" s="4">
+        <v>0.51</v>
+      </c>
+    </row>
+    <row r="14" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="A14" s="9" t="s">
+        <v>41</v>
+      </c>
+      <c r="B14" s="4">
+        <v>1.22</v>
+      </c>
+      <c r="C14" s="7">
+        <v>46.3</v>
+      </c>
+      <c r="D14" s="8">
+        <v>4</v>
+      </c>
+      <c r="E14" s="7">
+        <v>22.9</v>
+      </c>
+      <c r="F14" s="7">
+        <v>44.5</v>
+      </c>
+      <c r="G14" s="7">
+        <v>97.3</v>
+      </c>
+      <c r="H14" s="4"/>
+      <c r="I14" s="4">
+        <v>0.44</v>
+      </c>
+      <c r="J14" s="4">
+        <v>0.42</v>
+      </c>
+      <c r="K14" s="4">
+        <v>0.33</v>
+      </c>
+      <c r="L14" s="4">
+        <v>0.31</v>
+      </c>
+      <c r="M14" s="4">
+        <v>0.81</v>
+      </c>
+      <c r="N14" s="4">
+        <v>0.46</v>
+      </c>
+    </row>
+    <row r="15" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="A15" s="9" t="s">
+        <v>66</v>
+      </c>
+      <c r="B15" s="4">
+        <v>0.89</v>
+      </c>
+      <c r="C15" s="7">
+        <v>51.2</v>
+      </c>
+      <c r="D15" s="8">
+        <v>5</v>
+      </c>
+      <c r="E15" s="7">
+        <v>42.4</v>
+      </c>
+      <c r="F15" s="7">
+        <v>45.7</v>
+      </c>
+      <c r="G15" s="7">
+        <v>113.2</v>
+      </c>
+      <c r="H15" s="4"/>
+      <c r="I15" s="4">
+        <v>0.22</v>
+      </c>
+      <c r="J15" s="4">
+        <v>0.47</v>
+      </c>
+      <c r="K15" s="4">
+        <v>0.44</v>
+      </c>
+      <c r="L15" s="4">
+        <v>0.44</v>
+      </c>
+      <c r="M15" s="4">
+        <v>0.73</v>
+      </c>
+      <c r="N15" s="4">
+        <v>0.46</v>
+      </c>
+    </row>
+    <row r="16" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="A16" s="9" t="s">
+        <v>45</v>
+      </c>
+      <c r="B16" s="4">
+        <v>1.1399999999999999</v>
+      </c>
+      <c r="C16" s="7">
+        <v>55.1</v>
+      </c>
+      <c r="D16" s="8">
+        <v>5</v>
+      </c>
+      <c r="E16" s="7">
+        <v>14.6</v>
+      </c>
+      <c r="F16" s="7">
+        <v>22.8</v>
+      </c>
+      <c r="G16" s="7">
+        <v>101.4</v>
+      </c>
+      <c r="H16" s="4"/>
+      <c r="I16" s="4">
+        <v>0.39</v>
+      </c>
+      <c r="J16" s="4">
+        <v>0.52</v>
+      </c>
+      <c r="K16" s="4">
+        <v>0.44</v>
+      </c>
+      <c r="L16" s="4">
+        <v>0.1</v>
+      </c>
+      <c r="M16" s="4">
+        <v>0.79</v>
+      </c>
+      <c r="N16" s="4">
+        <v>0.45</v>
+      </c>
+    </row>
+    <row r="17" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A17" s="9" t="s">
+        <v>42</v>
+      </c>
+      <c r="B17" s="4">
+        <v>1.17</v>
+      </c>
+      <c r="C17" s="7">
+        <v>59.4</v>
+      </c>
+      <c r="D17" s="8">
+        <v>4</v>
+      </c>
+      <c r="E17" s="7">
+        <v>15.1</v>
+      </c>
+      <c r="F17" s="7">
+        <v>14.2</v>
+      </c>
+      <c r="G17" s="7">
+        <v>88.9</v>
+      </c>
+      <c r="H17" s="4"/>
+      <c r="I17" s="4">
+        <v>0.41</v>
+      </c>
+      <c r="J17" s="4">
+        <v>0.56999999999999995</v>
+      </c>
+      <c r="K17" s="4">
+        <v>0.33</v>
+      </c>
+      <c r="L17" s="4">
+        <v>0.03</v>
+      </c>
+      <c r="M17" s="4">
+        <v>0.86</v>
+      </c>
+      <c r="N17" s="4">
+        <v>0.44</v>
+      </c>
+    </row>
+    <row r="18" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A18" s="9" t="s">
+        <v>44</v>
+      </c>
+      <c r="B18" s="4">
+        <v>0.99</v>
+      </c>
+      <c r="C18" s="7">
+        <v>46.8</v>
+      </c>
+      <c r="D18" s="8">
+        <v>5</v>
+      </c>
+      <c r="E18" s="7">
+        <v>18</v>
+      </c>
+      <c r="F18" s="7">
+        <v>32.1</v>
+      </c>
+      <c r="G18" s="7">
+        <v>101.7</v>
+      </c>
+      <c r="H18" s="4"/>
+      <c r="I18" s="4">
+        <v>0.28999999999999998</v>
+      </c>
+      <c r="J18" s="4">
+        <v>0.42</v>
+      </c>
+      <c r="K18" s="4">
+        <v>0.44</v>
+      </c>
+      <c r="L18" s="4">
+        <v>0.19</v>
+      </c>
+      <c r="M18" s="4">
+        <v>0.79</v>
+      </c>
+      <c r="N18" s="4">
+        <v>0.43</v>
+      </c>
+    </row>
+    <row r="19" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A19" s="9" t="s">
+        <v>67</v>
+      </c>
+      <c r="B19" s="4">
+        <v>1.02</v>
+      </c>
+      <c r="C19" s="7">
+        <v>48.1</v>
+      </c>
+      <c r="D19" s="8">
+        <v>4</v>
+      </c>
+      <c r="E19" s="7">
+        <v>24.6</v>
+      </c>
+      <c r="F19" s="7">
+        <v>18.8</v>
+      </c>
+      <c r="G19" s="7">
+        <v>68.400000000000006</v>
+      </c>
+      <c r="H19" s="4"/>
+      <c r="I19" s="4">
+        <v>0.31</v>
+      </c>
+      <c r="J19" s="4">
+        <v>0.44</v>
+      </c>
+      <c r="K19" s="4">
+        <v>0.33</v>
+      </c>
+      <c r="L19" s="4">
+        <v>0.13</v>
+      </c>
+      <c r="M19" s="4">
+        <v>0.96</v>
+      </c>
+      <c r="N19" s="4">
+        <v>0.43</v>
+      </c>
+    </row>
+    <row r="20" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A20" s="9" t="s">
+        <v>48</v>
+      </c>
+      <c r="B20" s="4">
+        <v>0.56000000000000005</v>
+      </c>
+      <c r="C20" s="7">
+        <v>35.4</v>
+      </c>
+      <c r="D20" s="8">
+        <v>6</v>
+      </c>
+      <c r="E20" s="7">
+        <v>48</v>
+      </c>
+      <c r="F20" s="7">
+        <v>65.7</v>
+      </c>
+      <c r="G20" s="7">
+        <v>134.1</v>
+      </c>
+      <c r="H20" s="4"/>
+      <c r="I20" s="4">
+        <v>0</v>
+      </c>
+      <c r="J20" s="4">
+        <v>0.28999999999999998</v>
+      </c>
+      <c r="K20" s="4">
+        <v>0.56000000000000005</v>
+      </c>
+      <c r="L20" s="4">
+        <v>0.63</v>
+      </c>
+      <c r="M20" s="4">
+        <v>0.62</v>
+      </c>
+      <c r="N20" s="4">
+        <v>0.42</v>
+      </c>
+    </row>
+    <row r="21" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A21" s="9" t="s">
+        <v>56</v>
+      </c>
+      <c r="B21" s="4">
+        <v>0.71</v>
+      </c>
+      <c r="C21" s="7">
+        <v>26.1</v>
+      </c>
+      <c r="D21" s="8">
+        <v>3</v>
+      </c>
+      <c r="E21" s="7">
+        <v>58.1</v>
+      </c>
+      <c r="F21" s="7">
+        <v>79.900000000000006</v>
+      </c>
+      <c r="G21" s="7">
+        <v>101.2</v>
+      </c>
+      <c r="H21" s="4"/>
+      <c r="I21" s="4">
+        <v>0.1</v>
+      </c>
+      <c r="J21" s="4">
+        <v>0.17</v>
+      </c>
+      <c r="K21" s="4">
+        <v>0.22</v>
+      </c>
+      <c r="L21" s="4">
+        <v>0.79</v>
+      </c>
+      <c r="M21" s="4">
+        <v>0.79</v>
+      </c>
+      <c r="N21" s="4">
+        <v>0.42</v>
+      </c>
+    </row>
+    <row r="22" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A22" s="9" t="s">
+        <v>68</v>
+      </c>
+      <c r="B22" s="4">
+        <v>1.02</v>
+      </c>
+      <c r="C22" s="7">
+        <v>25</v>
+      </c>
+      <c r="D22" s="8">
+        <v>5</v>
+      </c>
+      <c r="E22" s="7">
+        <v>15.4</v>
+      </c>
+      <c r="F22" s="7">
+        <v>27.9</v>
+      </c>
+      <c r="G22" s="7">
+        <v>118</v>
+      </c>
+      <c r="H22" s="4"/>
+      <c r="I22" s="4">
+        <v>0.31</v>
+      </c>
+      <c r="J22" s="4">
+        <v>0.16</v>
+      </c>
+      <c r="K22" s="4">
+        <v>0.44</v>
+      </c>
+      <c r="L22" s="4">
+        <v>0.14000000000000001</v>
+      </c>
+      <c r="M22" s="4">
+        <v>0.7</v>
+      </c>
+      <c r="N22" s="4">
+        <v>0.35</v>
+      </c>
+    </row>
+    <row r="23" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A23" s="9" t="s">
+        <v>43</v>
+      </c>
+      <c r="B23" s="4">
+        <v>1.04</v>
+      </c>
+      <c r="C23" s="7">
+        <v>27.4</v>
+      </c>
+      <c r="D23" s="8">
+        <v>2</v>
+      </c>
+      <c r="E23" s="7">
+        <v>16.7</v>
+      </c>
+      <c r="F23" s="7">
+        <v>25.6</v>
+      </c>
+      <c r="G23" s="7">
+        <v>79.8</v>
+      </c>
+      <c r="H23" s="4"/>
+      <c r="I23" s="4">
+        <v>0.32</v>
+      </c>
+      <c r="J23" s="4">
+        <v>0.19</v>
+      </c>
+      <c r="K23" s="4">
+        <v>0.11</v>
+      </c>
+      <c r="L23" s="4">
+        <v>0.13</v>
+      </c>
+      <c r="M23" s="4">
+        <v>0.9</v>
+      </c>
+      <c r="N23" s="4">
+        <v>0.33</v>
+      </c>
+    </row>
+    <row r="24" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A24" s="9" t="s">
+        <v>58</v>
+      </c>
+      <c r="B24" s="4">
+        <v>0.76</v>
+      </c>
+      <c r="C24" s="7">
+        <v>17.100000000000001</v>
+      </c>
+      <c r="D24" s="8">
+        <v>2</v>
+      </c>
+      <c r="E24" s="7">
+        <v>55.3</v>
+      </c>
+      <c r="F24" s="7">
+        <v>71.7</v>
+      </c>
+      <c r="G24" s="7">
+        <v>154.6</v>
+      </c>
+      <c r="H24" s="4"/>
+      <c r="I24" s="4">
+        <v>0.14000000000000001</v>
+      </c>
+      <c r="J24" s="4">
+        <v>7.0000000000000007E-2</v>
+      </c>
+      <c r="K24" s="4">
+        <v>0.11</v>
+      </c>
+      <c r="L24" s="4">
+        <v>0.71</v>
+      </c>
+      <c r="M24" s="4">
+        <v>0.51</v>
+      </c>
+      <c r="N24" s="4">
+        <v>0.31</v>
+      </c>
+    </row>
+    <row r="25" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A25" s="9" t="s">
+        <v>52</v>
+      </c>
+      <c r="B25" s="4">
+        <v>0.91</v>
+      </c>
+      <c r="C25" s="7">
+        <v>37.200000000000003</v>
+      </c>
+      <c r="D25" s="8">
+        <v>2</v>
+      </c>
+      <c r="E25" s="7">
+        <v>17.100000000000001</v>
+      </c>
+      <c r="F25" s="7">
+        <v>28.7</v>
+      </c>
+      <c r="G25" s="7">
+        <v>122.9</v>
+      </c>
+      <c r="H25" s="4"/>
+      <c r="I25" s="4">
+        <v>0.24</v>
+      </c>
+      <c r="J25" s="4">
+        <v>0.31</v>
+      </c>
+      <c r="K25" s="4">
+        <v>0.11</v>
+      </c>
+      <c r="L25" s="4">
+        <v>0.16</v>
+      </c>
+      <c r="M25" s="4">
+        <v>0.68</v>
+      </c>
+      <c r="N25" s="4">
+        <v>0.3</v>
+      </c>
+    </row>
+    <row r="26" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A26" s="9" t="s">
+        <v>50</v>
+      </c>
+      <c r="B26" s="4">
+        <v>0.84</v>
+      </c>
+      <c r="C26" s="7">
+        <v>11.6</v>
+      </c>
+      <c r="D26" s="8">
+        <v>2</v>
+      </c>
+      <c r="E26" s="7">
+        <v>32.4</v>
+      </c>
+      <c r="F26" s="7">
+        <v>55.3</v>
+      </c>
+      <c r="G26" s="7">
+        <v>117.9</v>
+      </c>
+      <c r="H26" s="4"/>
+      <c r="I26" s="4">
+        <v>0.19</v>
+      </c>
+      <c r="J26" s="4">
+        <v>0</v>
+      </c>
+      <c r="K26" s="4">
+        <v>0.11</v>
+      </c>
+      <c r="L26" s="4">
+        <v>0.45</v>
+      </c>
+      <c r="M26" s="4">
+        <v>0.7</v>
+      </c>
+      <c r="N26" s="4">
+        <v>0.28999999999999998</v>
+      </c>
+    </row>
+    <row r="27" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A27" s="9" t="s">
+        <v>54</v>
+      </c>
+      <c r="B27" s="4">
+        <v>0.69</v>
+      </c>
+      <c r="C27" s="7">
+        <v>27.1</v>
+      </c>
+      <c r="D27" s="8">
+        <v>2</v>
+      </c>
+      <c r="E27" s="7">
+        <v>10</v>
+      </c>
+      <c r="F27" s="7">
+        <v>13.7</v>
+      </c>
+      <c r="G27" s="7">
+        <v>60.9</v>
+      </c>
+      <c r="H27" s="4"/>
+      <c r="I27" s="4">
+        <v>0.08</v>
+      </c>
+      <c r="J27" s="4">
+        <v>0.19</v>
+      </c>
+      <c r="K27" s="4">
+        <v>0.11</v>
+      </c>
+      <c r="L27" s="4">
+        <v>0</v>
+      </c>
+      <c r="M27" s="4">
+        <v>1</v>
+      </c>
+      <c r="N27" s="4">
+        <v>0.28000000000000003</v>
+      </c>
+    </row>
+    <row r="28" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A28" s="9" t="s">
+        <v>49</v>
+      </c>
+      <c r="B28" s="4">
+        <v>0.64</v>
+      </c>
+      <c r="C28" s="7">
+        <v>15.9</v>
+      </c>
+      <c r="D28" s="8">
+        <v>2</v>
+      </c>
+      <c r="E28" s="7">
+        <v>25.7</v>
+      </c>
+      <c r="F28" s="7">
+        <v>47.9</v>
+      </c>
+      <c r="G28" s="7">
+        <v>107.7</v>
+      </c>
+      <c r="H28" s="4"/>
+      <c r="I28" s="4">
+        <v>0.05</v>
+      </c>
+      <c r="J28" s="4">
+        <v>0.05</v>
+      </c>
+      <c r="K28" s="4">
+        <v>0.11</v>
+      </c>
+      <c r="L28" s="4">
+        <v>0.36</v>
+      </c>
+      <c r="M28" s="4">
+        <v>0.76</v>
+      </c>
+      <c r="N28" s="4">
+        <v>0.27</v>
+      </c>
+    </row>
+    <row r="29" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A29" s="9" t="s">
+        <v>55</v>
+      </c>
+      <c r="B29" s="4">
+        <v>0.76</v>
+      </c>
+      <c r="C29" s="7">
+        <v>17.600000000000001</v>
+      </c>
+      <c r="D29" s="8">
+        <v>1</v>
+      </c>
+      <c r="E29" s="7">
+        <v>48.4</v>
+      </c>
+      <c r="F29" s="7">
+        <v>63.4</v>
+      </c>
+      <c r="G29" s="7">
+        <v>182.9</v>
+      </c>
+      <c r="H29" s="4"/>
+      <c r="I29" s="4">
+        <v>0.14000000000000001</v>
+      </c>
+      <c r="J29" s="4">
+        <v>7.0000000000000007E-2</v>
+      </c>
+      <c r="K29" s="4">
+        <v>0</v>
+      </c>
+      <c r="L29" s="4">
+        <v>0.61</v>
+      </c>
+      <c r="M29" s="4">
+        <v>0.37</v>
+      </c>
+      <c r="N29" s="4">
+        <v>0.24</v>
+      </c>
+    </row>
+    <row r="30" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A30" s="9" t="s">
+        <v>53</v>
+      </c>
+      <c r="B30" s="4">
+        <v>0.64</v>
+      </c>
+      <c r="C30" s="7">
+        <v>16.3</v>
+      </c>
+      <c r="D30" s="8">
+        <v>2</v>
+      </c>
+      <c r="E30" s="7">
+        <v>16</v>
+      </c>
+      <c r="F30" s="7">
+        <v>29.1</v>
+      </c>
+      <c r="G30" s="7">
+        <v>102.3</v>
+      </c>
+      <c r="H30" s="4"/>
+      <c r="I30" s="4">
+        <v>0.05</v>
+      </c>
+      <c r="J30" s="4">
+        <v>0.06</v>
+      </c>
+      <c r="K30" s="4">
+        <v>0.11</v>
+      </c>
+      <c r="L30" s="4">
+        <v>0.15</v>
+      </c>
+      <c r="M30" s="4">
+        <v>0.79</v>
+      </c>
+      <c r="N30" s="4">
+        <v>0.23</v>
+      </c>
+    </row>
+    <row r="31" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A31" s="9" t="s">
+        <v>57</v>
+      </c>
+      <c r="B31" s="4">
+        <v>0.81</v>
+      </c>
+      <c r="C31" s="7">
+        <v>13.5</v>
+      </c>
+      <c r="D31" s="8">
+        <v>1</v>
+      </c>
+      <c r="E31" s="7">
+        <v>40</v>
+      </c>
+      <c r="F31" s="7">
+        <v>62.2</v>
+      </c>
+      <c r="G31" s="7">
+        <v>253.9</v>
+      </c>
+      <c r="H31" s="4"/>
+      <c r="I31" s="4">
+        <v>0.17</v>
+      </c>
+      <c r="J31" s="4">
+        <v>0.02</v>
+      </c>
+      <c r="K31" s="4">
+        <v>0</v>
+      </c>
+      <c r="L31" s="4">
+        <v>0.55000000000000004</v>
+      </c>
+      <c r="M31" s="4">
+        <v>0</v>
+      </c>
+      <c r="N31" s="4">
+        <v>0.15</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="2">
+    <mergeCell ref="B1:G1"/>
+    <mergeCell ref="I1:M1"/>
+  </mergeCells>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{825FB5F7-1E60-E34B-A606-3D3C4E31472C}">
   <dimension ref="A1:F31"/>
   <sheetViews>
@@ -2168,13 +3529,13 @@
       <selection activeCell="F15" sqref="F15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="25.1640625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="25.1640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>38</v>
       </c>
@@ -2182,7 +3543,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="2" spans="1:6">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>0</v>
       </c>
@@ -2196,7 +3557,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="3" spans="1:6">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>21</v>
       </c>
@@ -2210,7 +3571,7 @@
         <v>0.84590965646869898</v>
       </c>
     </row>
-    <row r="4" spans="1:6">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>16</v>
       </c>
@@ -2232,7 +3593,7 @@
         <v>2.8255213984115013E-2</v>
       </c>
     </row>
-    <row r="5" spans="1:6">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>19</v>
       </c>
@@ -2254,7 +3615,7 @@
         <v>2.7219448627508913E-2</v>
       </c>
     </row>
-    <row r="6" spans="1:6">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>22</v>
       </c>
@@ -2276,7 +3637,7 @@
         <v>1.446187608433902E-2</v>
       </c>
     </row>
-    <row r="7" spans="1:6">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>17</v>
       </c>
@@ -2298,7 +3659,7 @@
         <v>3.5891098482110362E-3</v>
       </c>
     </row>
-    <row r="8" spans="1:6">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>32</v>
       </c>
@@ -2320,7 +3681,7 @@
         <v>0.13774992930741803</v>
       </c>
     </row>
-    <row r="9" spans="1:6">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>18</v>
       </c>
@@ -2342,7 +3703,7 @@
         <v>5.326204404979995E-3</v>
       </c>
     </row>
-    <row r="10" spans="1:6">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>8</v>
       </c>
@@ -2364,7 +3725,7 @@
         <v>4.1866045509593941E-2</v>
       </c>
     </row>
-    <row r="11" spans="1:6">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>7</v>
       </c>
@@ -2386,7 +3747,7 @@
         <v>5.9335017389531064E-2</v>
       </c>
     </row>
-    <row r="12" spans="1:6">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>1</v>
       </c>
@@ -2408,7 +3769,7 @@
         <v>5.5640099236269336E-3</v>
       </c>
     </row>
-    <row r="13" spans="1:6">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>20</v>
       </c>
@@ -2430,7 +3791,7 @@
         <v>1.1611407277859032E-2</v>
       </c>
     </row>
-    <row r="14" spans="1:6">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>2</v>
       </c>
@@ -2452,7 +3813,7 @@
         <v>4.8095947082725021E-2</v>
       </c>
     </row>
-    <row r="15" spans="1:6">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>23</v>
       </c>
@@ -2474,7 +3835,7 @@
         <v>1.5952861731109991E-3</v>
       </c>
     </row>
-    <row r="16" spans="1:6">
+    <row r="16" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>24</v>
       </c>
@@ -2496,7 +3857,7 @@
         <v>1.2858621263365955E-2</v>
       </c>
     </row>
-    <row r="17" spans="1:6">
+    <row r="17" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
         <v>6</v>
       </c>
@@ -2518,7 +3879,7 @@
         <v>8.0131973691960345E-3</v>
       </c>
     </row>
-    <row r="18" spans="1:6">
+    <row r="18" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
         <v>3</v>
       </c>
@@ -2540,7 +3901,7 @@
         <v>7.793390053460969E-3</v>
       </c>
     </row>
-    <row r="19" spans="1:6">
+    <row r="19" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
         <v>5</v>
       </c>
@@ -2562,7 +3923,7 @@
         <v>6.2945606601580439E-3</v>
       </c>
     </row>
-    <row r="20" spans="1:6">
+    <row r="20" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
         <v>13</v>
       </c>
@@ -2584,7 +3945,7 @@
         <v>8.9368070802559596E-3</v>
       </c>
     </row>
-    <row r="21" spans="1:6">
+    <row r="21" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
         <v>33</v>
       </c>
@@ -2606,7 +3967,7 @@
         <v>7.6942524712803051E-4</v>
       </c>
     </row>
-    <row r="22" spans="1:6">
+    <row r="22" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
         <v>25</v>
       </c>
@@ -2628,7 +3989,7 @@
         <v>6.5407172693628002E-2</v>
       </c>
     </row>
-    <row r="23" spans="1:6">
+    <row r="23" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
         <v>4</v>
       </c>
@@ -2650,7 +4011,7 @@
         <v>2.0008564841407006E-2</v>
       </c>
     </row>
-    <row r="24" spans="1:6">
+    <row r="24" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
         <v>11</v>
       </c>
@@ -2672,7 +4033,7 @@
         <v>2.2631594061037985E-2</v>
       </c>
     </row>
-    <row r="25" spans="1:6">
+    <row r="25" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
         <v>15</v>
       </c>
@@ -2694,7 +4055,7 @@
         <v>1.0286459814579985E-2</v>
       </c>
     </row>
-    <row r="26" spans="1:6">
+    <row r="26" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
         <v>10</v>
       </c>
@@ -2716,7 +4077,7 @@
         <v>7.224130992630029E-3</v>
       </c>
     </row>
-    <row r="27" spans="1:6">
+    <row r="27" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
         <v>35</v>
       </c>
@@ -2738,7 +4099,7 @@
         <v>1.4761014993034005E-2</v>
       </c>
     </row>
-    <row r="28" spans="1:6">
+    <row r="28" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
         <v>9</v>
       </c>
@@ -2760,7 +4121,7 @@
         <v>1.0947785970282953E-2</v>
       </c>
     </row>
-    <row r="29" spans="1:6">
+    <row r="29" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
         <v>12</v>
       </c>
@@ -2782,7 +4143,7 @@
         <v>2.816974877368103E-2</v>
       </c>
     </row>
-    <row r="30" spans="1:6">
+    <row r="30" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
         <v>34</v>
       </c>
@@ -2804,7 +4165,7 @@
         <v>5.6142308733450053E-3</v>
       </c>
     </row>
-    <row r="31" spans="1:6">
+    <row r="31" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
         <v>14</v>
       </c>

</xml_diff>